<commit_message>
Updated tasks and hours
</commit_message>
<xml_diff>
--- a/bezpiecznik_godziny.xlsx
+++ b/bezpiecznik_godziny.xlsx
@@ -1,30 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wojtek\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\konra\Desktop\Bezpiecznik\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629FD15F-43D2-43A1-9CBF-0B9A8FCA66BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19752" windowHeight="6456"/>
+    <workbookView xWindow="2970" yWindow="135" windowWidth="23355" windowHeight="15645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="50">
   <si>
     <t>zadanie</t>
   </si>
@@ -140,9 +149,6 @@
     <t>Aktualizacja wyglądu</t>
   </si>
   <si>
-    <t>Implementacja statystyk</t>
-  </si>
-  <si>
     <t>Strona informacyjna</t>
   </si>
   <si>
@@ -168,12 +174,21 @@
   </si>
   <si>
     <t>Praca nad wyglądem siatki</t>
+  </si>
+  <si>
+    <t>Implementacja historii</t>
+  </si>
+  <si>
+    <t>Zmiany w adapterze histroii</t>
+  </si>
+  <si>
+    <t>Testy api oraz komunikacji telefonu z api</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -218,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -239,6 +254,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -535,29 +553,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="22.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="6"/>
-    <col min="8" max="8" width="15.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="1"/>
-    <col min="10" max="10" width="8.88671875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="22.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="6"/>
+    <col min="8" max="8" width="15.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="1"/>
+    <col min="10" max="10" width="8.85546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="J2" s="8" t="s">
         <v>30</v>
       </c>
@@ -568,7 +586,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -591,23 +609,23 @@
         <v>23</v>
       </c>
       <c r="J3" s="8">
-        <f>SUMIFS($F$4:$F$54,$D$4:$D$54,"Wojciech Kajstura")</f>
+        <f>SUMIFS($F$4:$F$56,$D$4:$D$56,"Wojciech Kajstura")</f>
         <v>115</v>
       </c>
       <c r="K3" s="8">
-        <f>SUMIFS($F$4:$F$54,$D$4:$D$54,"Konrad Lubera")</f>
-        <v>80</v>
+        <f>SUMIFS($F$4:$F$56,$D$4:$D$56,"Konrad Lubera")</f>
+        <v>114</v>
       </c>
       <c r="L3" s="8">
-        <f>SUMIFS($F$4:$F$54,$D$4:$D$54,"Remigiusz Drobinski")</f>
+        <f>SUMIFS($F$4:$F$56,$D$4:$D$56,"Remigiusz Drobinski")</f>
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -623,13 +641,13 @@
         <f t="shared" ref="G4:G32" si="0">(E4-F4)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="H4" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
@@ -643,11 +661,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
@@ -661,11 +679,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="12"/>
-      <c r="C7" s="12" t="s">
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -681,11 +699,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
@@ -699,11 +717,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="12"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="2" t="s">
         <v>10</v>
       </c>
@@ -717,11 +735,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="12"/>
-      <c r="C10" s="12" t="s">
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -737,11 +755,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
@@ -755,11 +773,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="12"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
@@ -773,11 +791,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="12"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12" t="s">
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="13"/>
+      <c r="C13" s="13" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -793,11 +811,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="12"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
@@ -811,11 +829,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="12"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="2" t="s">
         <v>10</v>
       </c>
@@ -829,13 +847,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H15" s="12"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="12" t="s">
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -851,13 +869,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
+      <c r="H16" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
       <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
@@ -871,11 +889,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
@@ -889,13 +907,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="12"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="12" t="s">
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="13" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -911,13 +929,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
+      <c r="H19" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
       <c r="D20" s="2" t="s">
         <v>9</v>
       </c>
@@ -931,11 +949,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H20" s="12"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
       <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
@@ -949,11 +967,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="12"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12" t="s">
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -969,11 +987,11 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="H22" s="12"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
+      <c r="H22" s="13"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
       <c r="D23" s="2" t="s">
         <v>9</v>
       </c>
@@ -987,11 +1005,11 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="H23" s="12"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
       <c r="D24" s="2" t="s">
         <v>10</v>
       </c>
@@ -1005,11 +1023,11 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="H24" s="12"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12" t="s">
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="13"/>
+      <c r="C25" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D25" s="2" t="s">
@@ -1025,11 +1043,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="12"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
       <c r="D26" s="2" t="s">
         <v>9</v>
       </c>
@@ -1043,11 +1061,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H26" s="12"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
       <c r="D27" s="2" t="s">
         <v>10</v>
       </c>
@@ -1061,9 +1079,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="12"/>
-    </row>
-    <row r="28" spans="2:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="2:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>20</v>
       </c>
@@ -1087,11 +1105,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="12" t="s">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D29" s="2" t="s">
@@ -1107,13 +1125,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
+      <c r="H29" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
       <c r="D30" s="2" t="s">
         <v>9</v>
       </c>
@@ -1127,11 +1145,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H30" s="12"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="2" t="s">
         <v>10</v>
       </c>
@@ -1145,9 +1163,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="12"/>
-    </row>
-    <row r="32" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1169,7 +1187,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>26</v>
       </c>
@@ -1191,7 +1209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>27</v>
       </c>
@@ -1203,17 +1221,17 @@
         <v>6</v>
       </c>
       <c r="F34" s="8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G34" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>28</v>
       </c>
@@ -1235,7 +1253,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
         <v>33</v>
       </c>
@@ -1257,7 +1275,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B37" s="10" t="s">
         <v>34</v>
       </c>
@@ -1279,7 +1297,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
         <v>35</v>
       </c>
@@ -1301,7 +1319,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
         <v>36</v>
       </c>
@@ -1323,7 +1341,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
         <v>37</v>
       </c>
@@ -1345,29 +1363,31 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="10" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E41" s="10">
-        <v>6</v>
-      </c>
-      <c r="F41" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="F41" s="10">
+        <v>20</v>
+      </c>
       <c r="G41" s="5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>-10</v>
       </c>
       <c r="H41" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
@@ -1387,9 +1407,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B43" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
@@ -1409,9 +1429,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="11" t="s">
@@ -1431,9 +1451,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11" t="s">
@@ -1453,9 +1473,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B46" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="11" t="s">
@@ -1475,9 +1495,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C47" s="11"/>
       <c r="D47" s="11" t="s">
@@ -1497,9 +1517,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C48" s="11"/>
       <c r="D48" s="11" t="s">
@@ -1519,57 +1539,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="11">
-        <v>4</v>
-      </c>
-      <c r="F49" s="11">
-        <v>5</v>
+    <row r="49" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B49" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="12">
+        <v>3</v>
+      </c>
+      <c r="F49" s="12">
+        <v>3</v>
       </c>
       <c r="G49" s="5">
         <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B50" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="11">
-        <v>4</v>
-      </c>
-      <c r="F50" s="11">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B50" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="12">
+        <v>7</v>
+      </c>
+      <c r="F50" s="12">
+        <v>7</v>
       </c>
       <c r="G50" s="5">
         <f t="shared" si="1"/>
-        <v>-1</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C51" s="11"/>
       <c r="D51" s="11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E51" s="11">
         <v>4</v>
@@ -1578,64 +1598,64 @@
         <v>5</v>
       </c>
       <c r="G51" s="5">
-        <f t="shared" si="1"/>
+        <f>(E51-F51)</f>
         <v>-1</v>
       </c>
       <c r="H51" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C52" s="11"/>
       <c r="D52" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E52" s="11">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F52" s="11">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G52" s="5">
-        <f t="shared" si="1"/>
-        <v>-2</v>
+        <f>(E52-F52)</f>
+        <v>-1</v>
       </c>
       <c r="H52" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C53" s="11"/>
       <c r="D53" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E53" s="11">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F53" s="11">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G53" s="5">
-        <f t="shared" si="1"/>
-        <v>-2</v>
+        <f>(E53-F53)</f>
+        <v>-1</v>
       </c>
       <c r="H53" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C54" s="11"/>
       <c r="D54" s="11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E54" s="11">
         <v>18</v>
@@ -1644,15 +1664,60 @@
         <v>20</v>
       </c>
       <c r="G54" s="5">
-        <f t="shared" si="1"/>
+        <f>(E54-F54)</f>
         <v>-2</v>
       </c>
       <c r="H54" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="11">
+        <v>18</v>
+      </c>
+      <c r="F55" s="11">
+        <v>20</v>
+      </c>
+      <c r="G55" s="5">
+        <f>(E55-F55)</f>
+        <v>-2</v>
+      </c>
+      <c r="H55" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="11">
+        <v>18</v>
+      </c>
+      <c r="F56" s="11">
+        <v>20</v>
+      </c>
+      <c r="G56" s="5">
+        <f>(E56-F56)</f>
+        <v>-2</v>
+      </c>
+      <c r="H56" s="11" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B19:B27"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="C25:C27"/>
@@ -1669,7 +1734,6 @@
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="C13:C15"/>
     <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>